<commit_message>
change css dowload statictis cv
</commit_message>
<xml_diff>
--- a/public/downloadCV/StatisticCV.xlsx
+++ b/public/downloadCV/StatisticCV.xlsx
@@ -22,19 +22,10 @@
     <t>Thống kê số lượng CV theo tháng trong năm 2016</t>
   </si>
   <si>
-    <t>tháng trong năm 2016</t>
-  </si>
-  <si>
-    <t>Số lượng CV update</t>
-  </si>
-  <si>
-    <t>Số lượng CV Pass</t>
-  </si>
-  <si>
-    <t>Tháng 4</t>
-  </si>
-  <si>
-    <t>Tháng 8</t>
+    <t>CV update</t>
+  </si>
+  <si>
+    <t>Tháng 3</t>
   </si>
   <si>
     <t>game development</t>
@@ -65,6 +56,15 @@
   </si>
   <si>
     <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Chế Hoàng Nghi</t>
+  </si>
+  <si>
+    <t>pma@example.org</t>
+  </si>
+  <si>
+    <t>Chờ duyệt</t>
   </si>
 </sst>
 </file>
@@ -157,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -166,9 +166,6 @@
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -476,63 +473,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="11.711426" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" customHeight="1" ht="30px">
+    <row r="1" spans="1:2" customHeight="1" ht="30px">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
@@ -554,37 +530,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="28.135986" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="28.135986" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="28.135986" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15px" customWidth="true" style="0"/>
+    <col min="3" max="3" width="15px" customWidth="true" style="0"/>
+    <col min="4" max="4" width="15px" customWidth="true" style="0"/>
+    <col min="5" max="5" width="15px" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15px" customWidth="true" style="0"/>
+    <col min="7" max="7" width="15px" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" customHeight="1" ht="30px">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" customHeight="1" ht="30px">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -593,79 +557,31 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -677,114 +593,19 @@
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0</v>
-      </c>
-      <c r="S4" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
@@ -806,19 +627,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="10px" customWidth="true" style="0"/>
+    <col min="2" max="2" width="20px" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customHeight="1" ht="30px">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -827,17 +649,34 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change css statistic CV
</commit_message>
<xml_diff>
--- a/public/downloadCV/StatisticCV.xlsx
+++ b/public/downloadCV/StatisticCV.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="mySheet" sheetId="1" r:id="rId4"/>
-    <sheet name="mySheet1" sheetId="2" r:id="rId5"/>
-    <sheet name="mySheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="Trạng thái" sheetId="1" r:id="rId4"/>
+    <sheet name="Chi Tiết" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -17,51 +16,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
-  <si>
-    <t>Thống kê số lượng CV theo tháng trong năm 2016</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+  <si>
+    <t>Thống kê số lượng CV theo Vị trí apply to</t>
   </si>
   <si>
     <t>CV update</t>
   </si>
   <si>
-    <t>Tháng 3</t>
-  </si>
-  <si>
-    <t>game development</t>
-  </si>
-  <si>
-    <t>smartphone applications</t>
-  </si>
-  <si>
-    <t>web applications</t>
-  </si>
-  <si>
-    <t>maintenance</t>
-  </si>
-  <si>
-    <t>dedicated team</t>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Vị trí</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Thái Mạnh Khánh</t>
+  </si>
+  <si>
+    <t>chung13@example.com</t>
   </si>
   <si>
     <t>portfolio</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Vị trí</t>
-  </si>
-  <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
-    <t>Chế Hoàng Nghi</t>
-  </si>
-  <si>
-    <t>pma@example.org</t>
   </si>
   <si>
     <t>Chờ duyệt</t>
@@ -481,7 +465,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="11.711426" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -530,103 +514,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="15px" customWidth="true" style="0"/>
-    <col min="3" max="3" width="15px" customWidth="true" style="0"/>
-    <col min="4" max="4" width="15px" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15px" customWidth="true" style="0"/>
-    <col min="6" max="6" width="15px" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15px" customWidth="true" style="0"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" customHeight="1" ht="30px">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
@@ -651,33 +538,33 @@
     <row r="2" spans="1:5">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="2">
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>